<commit_message>
fix PIVOT in quickSort
</commit_message>
<xml_diff>
--- a/cpp_lab2_4sem/newTest/new_graph.xlsx
+++ b/cpp_lab2_4sem/newTest/new_graph.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EC5844-7954-47EE-949E-22AFC5F24CD8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C5B698-75F5-437E-B8E9-A8FF74377B52}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insertSort" sheetId="1" r:id="rId1"/>
@@ -8209,8 +8209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView zoomScale="51" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8218,7 +8218,7 @@
     <col min="2" max="2" width="20.90625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="19.08984375" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -8822,8 +8822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26DE728-B3D5-4302-A44B-F3E7162CB082}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="35" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>